<commit_message>
can direct 버그 수정
</commit_message>
<xml_diff>
--- a/시리얼 통신 프로토콜 패킷 정의 ver 1.5.xlsx
+++ b/시리얼 통신 프로토콜 패킷 정의 ver 1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\VINE\eti\Software\rev1\CAN_TO_SER_ASCII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA95D54-D8A1-4E7F-BA0E-2ED16C171A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2014330-5680-487B-BC6C-D6F76743E8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="21915" windowHeight="13950" xr2:uid="{E66AFE45-41E1-4BAD-ABE0-FAC778471578}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="22890" windowHeight="12615" xr2:uid="{E66AFE45-41E1-4BAD-ABE0-FAC778471578}"/>
   </bookViews>
   <sheets>
     <sheet name="기본패킷구조" sheetId="1" r:id="rId1"/>
@@ -1048,13 +1048,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1072,15 +1081,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907009A8-511E-4F0D-929F-8D98B6E0DC45}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="I28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1851,13 +1851,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
@@ -1877,11 +1877,11 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="7">
         <v>1</v>
       </c>
@@ -1906,38 +1906,38 @@
       <c r="M2" s="7">
         <v>8</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="24" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="19"/>
+      <c r="L3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="25"/>
+      <c r="M3" s="19"/>
       <c r="N3" s="8" t="s">
         <v>22</v>
       </c>
@@ -1961,42 +1961,42 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="20"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="23"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="7">
         <v>1</v>
       </c>
@@ -2033,41 +2033,41 @@
       <c r="Q5" s="7">
         <v>12</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="23"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="26"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="24" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="25" t="s">
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25" t="s">
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
       <c r="R6" s="8" t="s">
         <v>33</v>
       </c>
@@ -2094,13 +2094,13 @@
       </c>
     </row>
     <row r="7" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="16" t="s">
         <v>16</v>
       </c>
@@ -2112,11 +2112,11 @@
       <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:25" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="7" t="s">
         <v>37</v>
       </c>
@@ -2129,13 +2129,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="F1:T1"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
     <mergeCell ref="A7:E8"/>
     <mergeCell ref="F7:L7"/>
     <mergeCell ref="A4:E6"/>
@@ -2144,6 +2137,13 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="F1:T1"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>